<commit_message>
spreadsheet for parameter exploration was added
</commit_message>
<xml_diff>
--- a/summary/dimension_numbers.xlsx
+++ b/summary/dimension_numbers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kourosh_hakhamaneshi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kourosh_hakhamaneshi/Documents/dev/deep_ckt_workspace/autoreg_ckt/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A5E67C-1D73-1A4E-B0CE-FAB91AB3135C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ECEA7C-88D9-564B-9189-F39E70D2A7A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="14080" windowHeight="17540" activeTab="1" xr2:uid="{8BABC831-9994-DE4A-B0FB-3CC74B289DE6}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="28120" windowHeight="17540" activeTab="1" xr2:uid="{8BABC831-9994-DE4A-B0FB-3CC74B289DE6}"/>
   </bookViews>
   <sheets>
     <sheet name="ackley" sheetId="1" r:id="rId1"/>
@@ -464,9 +464,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -547,6 +544,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1052,7 +1052,7 @@
       </c>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
@@ -1060,13 +1060,13 @@
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="8"/>
+      <c r="C11" s="47"/>
       <c r="D11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="47" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
@@ -1074,13 +1074,13 @@
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C14" s="8"/>
+      <c r="C14" s="47"/>
       <c r="D14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="47" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
@@ -1088,7 +1088,7 @@
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="8"/>
+      <c r="C17" s="47"/>
       <c r="D17" t="s">
         <v>1</v>
       </c>
@@ -1107,78 +1107,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C24198-D24B-1E4D-91F5-5ADF80A79CF3}">
   <dimension ref="C1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19.6640625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="12" style="17" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="23" customWidth="1"/>
-    <col min="9" max="10" width="12.33203125" style="30" customWidth="1"/>
-    <col min="11" max="12" width="12.83203125" style="30" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="30" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="30" customWidth="1"/>
-    <col min="15" max="15" width="12" style="30" customWidth="1"/>
-    <col min="16" max="17" width="10.83203125" style="30"/>
-    <col min="18" max="20" width="10.83203125" style="38"/>
-    <col min="21" max="23" width="10.83203125" style="30"/>
-    <col min="24" max="26" width="10.83203125" style="38"/>
+    <col min="5" max="6" width="10.83203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="12" style="16" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="22" customWidth="1"/>
+    <col min="9" max="10" width="12.33203125" style="29" customWidth="1"/>
+    <col min="11" max="12" width="12.83203125" style="29" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="29" customWidth="1"/>
+    <col min="14" max="14" width="11.5" style="29" customWidth="1"/>
+    <col min="15" max="15" width="12" style="29" customWidth="1"/>
+    <col min="16" max="17" width="10.83203125" style="29"/>
+    <col min="18" max="20" width="10.83203125" style="37"/>
+    <col min="21" max="23" width="10.83203125" style="29"/>
+    <col min="24" max="26" width="10.83203125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W1" s="33"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
     </row>
     <row r="2" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W2" s="33"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
     </row>
     <row r="3" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W3" s="33"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="42"/>
     </row>
     <row r="4" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W4" s="33"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
     </row>
     <row r="5" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W5" s="33"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="42"/>
+      <c r="Y5" s="42"/>
+      <c r="Z5" s="42"/>
     </row>
     <row r="6" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="S6" s="38">
+      <c r="S6" s="37">
         <v>3</v>
       </c>
-      <c r="T6" s="38">
+      <c r="T6" s="37">
         <v>4</v>
       </c>
-      <c r="V6" s="30">
+      <c r="V6" s="29">
         <v>1</v>
       </c>
-      <c r="W6" s="33">
+      <c r="W6" s="32">
         <v>2</v>
       </c>
-      <c r="X6" s="43">
+      <c r="X6" s="42">
         <v>5</v>
       </c>
-      <c r="Y6" s="43">
+      <c r="Y6" s="42">
         <v>6</v>
       </c>
-      <c r="Z6" s="43">
+      <c r="Z6" s="42">
         <v>7</v>
       </c>
     </row>
@@ -1186,70 +1186,70 @@
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>2</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>5</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="21">
         <v>10</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="26">
         <v>20</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="26">
         <v>20</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="26">
         <v>20</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="26">
         <v>20</v>
       </c>
-      <c r="M7" s="27">
+      <c r="M7" s="26">
         <v>20</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="26">
         <v>20</v>
       </c>
-      <c r="O7" s="27">
+      <c r="O7" s="26">
         <v>20</v>
       </c>
-      <c r="P7" s="27">
+      <c r="P7" s="26">
         <v>20</v>
       </c>
-      <c r="Q7" s="27">
+      <c r="Q7" s="26">
         <v>20</v>
       </c>
-      <c r="R7" s="39">
+      <c r="R7" s="38">
         <v>20</v>
       </c>
-      <c r="S7" s="39">
+      <c r="S7" s="38">
         <v>20</v>
       </c>
-      <c r="T7" s="39">
+      <c r="T7" s="38">
         <v>20</v>
       </c>
-      <c r="U7" s="27">
+      <c r="U7" s="26">
         <v>20</v>
       </c>
-      <c r="V7" s="27">
+      <c r="V7" s="26">
         <v>20</v>
       </c>
-      <c r="W7" s="34">
+      <c r="W7" s="33">
         <v>20</v>
       </c>
-      <c r="X7" s="44">
+      <c r="X7" s="43">
         <v>20</v>
       </c>
-      <c r="Y7" s="44">
+      <c r="Y7" s="43">
         <v>20</v>
       </c>
-      <c r="Z7" s="44">
+      <c r="Z7" s="43">
         <v>20</v>
       </c>
     </row>
@@ -1257,70 +1257,70 @@
       <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="K8" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="N8" s="30" t="s">
+      <c r="N8" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="O8" s="28" t="s">
+      <c r="O8" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="P8" s="28" t="s">
+      <c r="P8" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="Q8" s="28" t="s">
+      <c r="Q8" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="R8" s="40" t="s">
+      <c r="R8" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="S8" s="40" t="s">
+      <c r="S8" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="T8" s="40" t="s">
+      <c r="T8" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="U8" s="28" t="s">
+      <c r="U8" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="V8" s="28" t="s">
+      <c r="V8" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="W8" s="35" t="s">
+      <c r="W8" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="X8" s="45" t="s">
+      <c r="X8" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="Y8" s="45" t="s">
+      <c r="Y8" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="Z8" s="45" t="s">
+      <c r="Z8" s="44" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1328,70 +1328,70 @@
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>5</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>5</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <v>5</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="23">
         <v>5</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="30">
         <v>5</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="30">
         <v>5</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="30">
         <v>10</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="30">
         <v>40</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="30">
         <v>40</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="30">
         <v>40</v>
       </c>
-      <c r="O9" s="31">
+      <c r="O9" s="30">
         <v>40</v>
       </c>
-      <c r="P9" s="31">
+      <c r="P9" s="30">
         <v>40</v>
       </c>
-      <c r="Q9" s="31">
+      <c r="Q9" s="30">
         <v>40</v>
       </c>
-      <c r="R9" s="41">
+      <c r="R9" s="40">
         <v>5</v>
       </c>
-      <c r="S9" s="41">
+      <c r="S9" s="40">
         <v>5</v>
       </c>
-      <c r="T9" s="41">
+      <c r="T9" s="40">
         <v>5</v>
       </c>
-      <c r="U9" s="31">
+      <c r="U9" s="30">
         <v>40</v>
       </c>
-      <c r="V9" s="31">
+      <c r="V9" s="30">
         <v>40</v>
       </c>
-      <c r="W9" s="36">
+      <c r="W9" s="35">
         <v>40</v>
       </c>
-      <c r="X9" s="46">
+      <c r="X9" s="45">
         <v>40</v>
       </c>
-      <c r="Y9" s="46">
+      <c r="Y9" s="45">
         <v>40</v>
       </c>
-      <c r="Z9" s="46">
+      <c r="Z9" s="45">
         <v>40</v>
       </c>
     </row>
@@ -1399,70 +1399,70 @@
       <c r="C10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>1</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>1</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>1</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="23">
         <v>1</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="30">
         <v>1</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="30">
         <v>1</v>
       </c>
-      <c r="K10" s="31">
+      <c r="K10" s="30">
         <v>1</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="30">
         <v>1</v>
       </c>
-      <c r="M10" s="31">
+      <c r="M10" s="30">
         <v>1</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="30">
         <v>1</v>
       </c>
-      <c r="O10" s="31">
+      <c r="O10" s="30">
         <v>1</v>
       </c>
-      <c r="P10" s="31">
+      <c r="P10" s="30">
         <v>1</v>
       </c>
-      <c r="Q10" s="31">
+      <c r="Q10" s="30">
         <v>1</v>
       </c>
-      <c r="R10" s="41">
+      <c r="R10" s="40">
         <v>10</v>
       </c>
-      <c r="S10" s="41">
+      <c r="S10" s="40">
         <v>10</v>
       </c>
-      <c r="T10" s="41">
+      <c r="T10" s="40">
         <v>10</v>
       </c>
-      <c r="U10" s="31">
+      <c r="U10" s="30">
         <v>10</v>
       </c>
-      <c r="V10" s="31">
+      <c r="V10" s="30">
         <v>10</v>
       </c>
-      <c r="W10" s="36">
+      <c r="W10" s="35">
         <v>10</v>
       </c>
-      <c r="X10" s="46">
+      <c r="X10" s="45">
         <v>5</v>
       </c>
-      <c r="Y10" s="46">
+      <c r="Y10" s="45">
         <v>5</v>
       </c>
-      <c r="Z10" s="46">
+      <c r="Z10" s="45">
         <v>5</v>
       </c>
     </row>
@@ -1470,70 +1470,70 @@
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>10</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>20</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>10</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="23">
         <v>10</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="30">
         <v>10</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J11" s="29">
         <v>20</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K11" s="29">
         <v>10</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="30">
         <v>10</v>
       </c>
-      <c r="M11" s="31">
+      <c r="M11" s="30">
         <v>20</v>
       </c>
-      <c r="N11" s="31">
+      <c r="N11" s="30">
         <v>30</v>
       </c>
-      <c r="O11" s="31">
+      <c r="O11" s="30">
         <v>10</v>
       </c>
-      <c r="P11" s="31">
+      <c r="P11" s="30">
         <v>20</v>
       </c>
-      <c r="Q11" s="31">
+      <c r="Q11" s="30">
         <v>30</v>
       </c>
-      <c r="R11" s="41">
+      <c r="R11" s="40">
         <v>10</v>
       </c>
-      <c r="S11" s="41">
+      <c r="S11" s="40">
         <v>20</v>
       </c>
-      <c r="T11" s="41">
+      <c r="T11" s="40">
         <v>30</v>
       </c>
-      <c r="U11" s="31">
+      <c r="U11" s="30">
         <v>10</v>
       </c>
-      <c r="V11" s="31">
+      <c r="V11" s="30">
         <v>20</v>
       </c>
-      <c r="W11" s="36">
+      <c r="W11" s="35">
         <v>30</v>
       </c>
-      <c r="X11" s="46">
+      <c r="X11" s="45">
         <v>10</v>
       </c>
-      <c r="Y11" s="46">
+      <c r="Y11" s="45">
         <v>20</v>
       </c>
-      <c r="Z11" s="46">
+      <c r="Z11" s="45">
         <v>30</v>
       </c>
     </row>
@@ -1541,70 +1541,70 @@
       <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>150</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>150</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <v>500</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="23">
         <v>100</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="30">
         <v>1700</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="30">
         <v>1700</v>
       </c>
-      <c r="K12" s="31">
+      <c r="K12" s="30">
         <v>1700</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="30">
         <v>1700</v>
       </c>
-      <c r="M12" s="31">
+      <c r="M12" s="30">
         <v>1700</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="30">
         <v>1700</v>
       </c>
-      <c r="O12" s="31">
+      <c r="O12" s="30">
         <v>1700</v>
       </c>
-      <c r="P12" s="31">
+      <c r="P12" s="30">
         <v>1700</v>
       </c>
-      <c r="Q12" s="31">
+      <c r="Q12" s="30">
         <v>1700</v>
       </c>
-      <c r="R12" s="41">
+      <c r="R12" s="40">
         <v>1700</v>
       </c>
-      <c r="S12" s="41">
+      <c r="S12" s="40">
         <v>1700</v>
       </c>
-      <c r="T12" s="41">
+      <c r="T12" s="40">
         <v>1700</v>
       </c>
-      <c r="U12" s="31">
+      <c r="U12" s="30">
         <v>1700</v>
       </c>
-      <c r="V12" s="31">
+      <c r="V12" s="30">
         <v>1700</v>
       </c>
-      <c r="W12" s="36">
+      <c r="W12" s="35">
         <v>1700</v>
       </c>
-      <c r="X12" s="46">
+      <c r="X12" s="45">
         <v>1700</v>
       </c>
-      <c r="Y12" s="46">
+      <c r="Y12" s="45">
         <v>1700</v>
       </c>
-      <c r="Z12" s="46">
+      <c r="Z12" s="45">
         <v>1700</v>
       </c>
     </row>
@@ -1612,1429 +1612,1429 @@
       <c r="C13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>100</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="18">
+      <c r="F13" s="10"/>
+      <c r="G13" s="17">
         <v>2000</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="23">
         <v>1000</v>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="46"/>
-      <c r="Y13" s="46"/>
-      <c r="Z13" s="46"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="35"/>
+      <c r="X13" s="45"/>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="45"/>
     </row>
     <row r="14" spans="3:26" ht="17" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>100</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="18">
+      <c r="F14" s="10"/>
+      <c r="G14" s="17">
         <v>1000</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="23">
         <v>1000</v>
       </c>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="46"/>
-      <c r="Z14" s="46"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="35"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="45"/>
     </row>
     <row r="15" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W15" s="33"/>
-      <c r="X15" s="43"/>
-      <c r="Y15" s="43"/>
-      <c r="Z15" s="43"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="42"/>
+      <c r="Y15" s="42"/>
+      <c r="Z15" s="42"/>
     </row>
     <row r="16" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="47" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="23">
-        <v>0</v>
-      </c>
-      <c r="I16" s="30">
-        <v>0</v>
-      </c>
-      <c r="J16" s="30">
-        <v>0</v>
-      </c>
-      <c r="K16" s="30">
-        <v>0</v>
-      </c>
-      <c r="L16" s="30">
-        <v>0</v>
-      </c>
-      <c r="M16" s="30">
-        <v>0</v>
-      </c>
-      <c r="N16" s="30">
-        <v>0</v>
-      </c>
-      <c r="O16" s="30">
-        <v>0</v>
-      </c>
-      <c r="P16" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="30">
-        <v>0</v>
-      </c>
-      <c r="R16" s="38">
-        <v>0</v>
-      </c>
-      <c r="S16" s="38">
-        <v>0</v>
-      </c>
-      <c r="T16" s="38">
-        <v>0</v>
-      </c>
-      <c r="U16" s="30">
-        <v>0</v>
-      </c>
-      <c r="V16" s="30">
-        <v>0</v>
-      </c>
-      <c r="W16" s="33">
-        <v>0</v>
-      </c>
-      <c r="X16" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="43">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="43">
+      <c r="H16" s="22">
+        <v>0</v>
+      </c>
+      <c r="I16" s="29">
+        <v>0</v>
+      </c>
+      <c r="J16" s="29">
+        <v>0</v>
+      </c>
+      <c r="K16" s="29">
+        <v>0</v>
+      </c>
+      <c r="L16" s="29">
+        <v>0</v>
+      </c>
+      <c r="M16" s="29">
+        <v>0</v>
+      </c>
+      <c r="N16" s="29">
+        <v>0</v>
+      </c>
+      <c r="O16" s="29">
+        <v>0</v>
+      </c>
+      <c r="P16" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="29">
+        <v>0</v>
+      </c>
+      <c r="R16" s="37">
+        <v>0</v>
+      </c>
+      <c r="S16" s="37">
+        <v>0</v>
+      </c>
+      <c r="T16" s="37">
+        <v>0</v>
+      </c>
+      <c r="U16" s="29">
+        <v>0</v>
+      </c>
+      <c r="V16" s="29">
+        <v>0</v>
+      </c>
+      <c r="W16" s="32">
+        <v>0</v>
+      </c>
+      <c r="X16" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C17" s="8"/>
+      <c r="C17" s="47"/>
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="30" t="s">
+      <c r="J17" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="30" t="s">
+      <c r="K17" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="30" t="s">
+      <c r="L17" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="M17" s="30" t="s">
+      <c r="M17" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="N17" s="30" t="s">
+      <c r="N17" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="O17" s="28" t="s">
+      <c r="O17" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P17" s="28" t="s">
+      <c r="P17" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="28" t="s">
+      <c r="Q17" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="R17" s="40" t="s">
+      <c r="R17" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="S17" s="40" t="s">
+      <c r="S17" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="T17" s="40" t="s">
+      <c r="T17" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="U17" s="28" t="s">
+      <c r="U17" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="V17" s="28" t="s">
+      <c r="V17" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="W17" s="28" t="s">
+      <c r="W17" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="X17" s="40" t="s">
+      <c r="X17" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="Y17" s="40" t="s">
+      <c r="Y17" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="Z17" s="40" t="s">
+      <c r="Z17" s="39" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C18" s="8"/>
+      <c r="C18" s="47"/>
       <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="23">
-        <v>0</v>
-      </c>
-      <c r="W18" s="33"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="43"/>
-      <c r="Z18" s="43"/>
+      <c r="H18" s="22">
+        <v>0</v>
+      </c>
+      <c r="W18" s="32"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42"/>
     </row>
     <row r="19" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="8"/>
+      <c r="C19" s="47"/>
       <c r="D19" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="23">
-        <v>0</v>
-      </c>
-      <c r="W19" s="33"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="43"/>
-      <c r="Z19" s="43"/>
+      <c r="H19" s="22">
+        <v>0</v>
+      </c>
+      <c r="W19" s="32"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
     </row>
     <row r="20" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W20" s="33"/>
-      <c r="X20" s="43"/>
-      <c r="Y20" s="43"/>
-      <c r="Z20" s="43"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="42"/>
+      <c r="Y20" s="42"/>
+      <c r="Z20" s="42"/>
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="47" t="s">
         <v>57</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>5.4</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="16">
         <v>0.1</v>
       </c>
-      <c r="H21" s="23">
-        <v>0</v>
-      </c>
-      <c r="I21" s="30">
-        <v>0</v>
-      </c>
-      <c r="J21" s="30">
-        <v>0</v>
-      </c>
-      <c r="K21" s="30">
-        <v>0</v>
-      </c>
-      <c r="L21" s="30">
-        <v>0</v>
-      </c>
-      <c r="M21" s="30">
-        <v>0</v>
-      </c>
-      <c r="N21" s="30">
-        <v>0</v>
-      </c>
-      <c r="O21" s="30">
-        <v>0</v>
-      </c>
-      <c r="P21" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="30">
-        <v>0</v>
-      </c>
-      <c r="R21" s="38">
-        <v>0</v>
-      </c>
-      <c r="S21" s="38">
-        <v>0</v>
-      </c>
-      <c r="T21" s="38">
-        <v>0</v>
-      </c>
-      <c r="U21" s="30">
-        <v>0</v>
-      </c>
-      <c r="V21" s="30">
-        <v>0</v>
-      </c>
-      <c r="W21" s="33">
-        <v>0</v>
-      </c>
-      <c r="X21" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="43">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="43">
+      <c r="H21" s="22">
+        <v>0</v>
+      </c>
+      <c r="I21" s="29">
+        <v>0</v>
+      </c>
+      <c r="J21" s="29">
+        <v>0</v>
+      </c>
+      <c r="K21" s="29">
+        <v>0</v>
+      </c>
+      <c r="L21" s="29">
+        <v>0</v>
+      </c>
+      <c r="M21" s="29">
+        <v>0</v>
+      </c>
+      <c r="N21" s="29">
+        <v>0</v>
+      </c>
+      <c r="O21" s="29">
+        <v>0</v>
+      </c>
+      <c r="P21" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="29">
+        <v>0</v>
+      </c>
+      <c r="R21" s="37">
+        <v>0</v>
+      </c>
+      <c r="S21" s="37">
+        <v>0</v>
+      </c>
+      <c r="T21" s="37">
+        <v>0</v>
+      </c>
+      <c r="U21" s="29">
+        <v>0</v>
+      </c>
+      <c r="V21" s="29">
+        <v>0</v>
+      </c>
+      <c r="W21" s="32">
+        <v>0</v>
+      </c>
+      <c r="X21" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C22" s="8"/>
+      <c r="C22" s="47"/>
       <c r="D22" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>77.89</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="11">
         <v>88.1</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="18">
         <v>86.3</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="22">
         <v>70.599999999999994</v>
       </c>
-      <c r="I22" s="30">
+      <c r="I22" s="29">
         <v>0.4</v>
       </c>
-      <c r="J22" s="30">
+      <c r="J22" s="29">
         <v>39.1</v>
       </c>
-      <c r="K22" s="30">
+      <c r="K22" s="29">
         <v>44.7</v>
       </c>
-      <c r="L22" s="30">
+      <c r="L22" s="29">
         <v>9.8000000000000007</v>
       </c>
-      <c r="M22" s="30">
+      <c r="M22" s="29">
         <v>11.8</v>
       </c>
-      <c r="N22" s="30">
+      <c r="N22" s="29">
         <v>22.7</v>
       </c>
-      <c r="O22" s="28">
+      <c r="O22" s="27">
         <v>84.6</v>
       </c>
-      <c r="P22" s="28">
+      <c r="P22" s="27">
         <v>76.7</v>
       </c>
-      <c r="Q22" s="28">
+      <c r="Q22" s="27">
         <v>85.5</v>
       </c>
-      <c r="R22" s="40">
+      <c r="R22" s="39">
         <v>60</v>
       </c>
-      <c r="S22" s="40">
+      <c r="S22" s="39">
         <v>92</v>
       </c>
-      <c r="T22" s="40">
+      <c r="T22" s="39">
         <v>78</v>
       </c>
-      <c r="U22" s="28">
+      <c r="U22" s="27">
         <v>83</v>
       </c>
-      <c r="V22" s="28">
+      <c r="V22" s="27">
         <v>90.33</v>
       </c>
-      <c r="W22" s="35">
+      <c r="W22" s="34">
         <v>86.33</v>
       </c>
-      <c r="X22" s="45">
+      <c r="X22" s="44">
         <v>80</v>
       </c>
-      <c r="Y22" s="45">
+      <c r="Y22" s="44">
         <v>83</v>
       </c>
-      <c r="Z22" s="45">
+      <c r="Z22" s="44">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C23" s="8"/>
+      <c r="C23" s="47"/>
       <c r="D23" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>31.9</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>15.56</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="16">
         <v>4.9000000000000004</v>
       </c>
-      <c r="H23" s="23">
-        <v>0</v>
-      </c>
-      <c r="W23" s="33"/>
-      <c r="X23" s="43"/>
-      <c r="Y23" s="43"/>
-      <c r="Z23" s="43"/>
+      <c r="H23" s="22">
+        <v>0</v>
+      </c>
+      <c r="W23" s="32"/>
+      <c r="X23" s="42"/>
+      <c r="Y23" s="42"/>
+      <c r="Z23" s="42"/>
     </row>
     <row r="24" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="8"/>
+      <c r="C24" s="47"/>
       <c r="D24" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>85.5</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="9">
         <v>6.9</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="16">
         <v>55.5</v>
       </c>
-      <c r="H24" s="23">
-        <v>0</v>
-      </c>
-      <c r="W24" s="33"/>
-      <c r="X24" s="43"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="43"/>
+      <c r="H24" s="22">
+        <v>0</v>
+      </c>
+      <c r="W24" s="32"/>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="42"/>
     </row>
     <row r="25" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="2"/>
-      <c r="W25" s="33"/>
-      <c r="X25" s="43"/>
-      <c r="Y25" s="43"/>
-      <c r="Z25" s="43"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="42"/>
+      <c r="Z25" s="42"/>
     </row>
     <row r="26" spans="3:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="47" t="s">
         <v>3</v>
       </c>
       <c r="D26" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="9">
         <v>3.9169999999999998</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="9">
         <v>2.4</v>
       </c>
-      <c r="G26" s="17">
-        <v>0</v>
-      </c>
-      <c r="H26" s="23" t="s">
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+      <c r="H26" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="J26" s="30" t="s">
+      <c r="J26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="K26" s="30" t="s">
+      <c r="K26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="L26" s="30" t="s">
+      <c r="L26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="30" t="s">
+      <c r="M26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="N26" s="30" t="s">
+      <c r="N26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="O26" s="30" t="s">
+      <c r="O26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P26" s="30" t="s">
+      <c r="P26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="Q26" s="30" t="s">
+      <c r="Q26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="R26" s="38" t="s">
+      <c r="R26" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="S26" s="38" t="s">
+      <c r="S26" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="T26" s="38" t="s">
+      <c r="T26" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="U26" s="30" t="s">
+      <c r="U26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="V26" s="30" t="s">
+      <c r="V26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="W26" s="33" t="s">
+      <c r="W26" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="X26" s="43" t="s">
+      <c r="X26" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="Y26" s="43" t="s">
+      <c r="Y26" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="Z26" s="43" t="s">
+      <c r="Z26" s="42" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C27" s="8"/>
+      <c r="C27" s="47"/>
       <c r="D27" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="9">
         <v>7.64</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="9">
         <v>2.97</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G27" s="16">
         <v>2.4</v>
       </c>
-      <c r="H27" s="23">
+      <c r="H27" s="22">
         <v>2.4700000000000002</v>
       </c>
-      <c r="I27" s="30">
+      <c r="I27" s="29">
         <v>0.75</v>
       </c>
-      <c r="J27" s="30">
+      <c r="J27" s="29">
         <v>2.79</v>
       </c>
-      <c r="K27" s="30">
+      <c r="K27" s="29">
         <v>0.8</v>
       </c>
-      <c r="L27" s="30">
+      <c r="L27" s="29">
         <v>0.92</v>
       </c>
-      <c r="M27" s="30">
+      <c r="M27" s="29">
         <v>2.048</v>
       </c>
-      <c r="N27" s="30">
+      <c r="N27" s="29">
         <v>1.58</v>
       </c>
-      <c r="O27" s="30">
+      <c r="O27" s="29">
         <v>1.17</v>
       </c>
-      <c r="P27" s="30">
+      <c r="P27" s="29">
         <v>1.23</v>
       </c>
-      <c r="Q27" s="30">
+      <c r="Q27" s="29">
         <v>1.5</v>
       </c>
-      <c r="R27" s="38">
+      <c r="R27" s="37">
         <v>1.95</v>
       </c>
-      <c r="S27" s="38">
+      <c r="S27" s="37">
         <v>1.74</v>
       </c>
-      <c r="T27" s="38">
+      <c r="T27" s="37">
         <v>1.1299999999999999</v>
       </c>
-      <c r="U27" s="30">
+      <c r="U27" s="29">
         <v>1.29</v>
       </c>
-      <c r="V27" s="30">
+      <c r="V27" s="29">
         <v>2.278</v>
       </c>
-      <c r="W27" s="33">
+      <c r="W27" s="32">
         <v>1.577</v>
       </c>
-      <c r="X27" s="43">
+      <c r="X27" s="42">
         <v>1.8520000000000001</v>
       </c>
-      <c r="Y27" s="43">
+      <c r="Y27" s="42">
         <v>0.96</v>
       </c>
-      <c r="Z27" s="43">
+      <c r="Z27" s="42">
         <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="28" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C28" s="8"/>
+      <c r="C28" s="47"/>
       <c r="D28" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="9">
         <v>1.72</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="9">
         <v>4.3</v>
       </c>
-      <c r="G28" s="17">
+      <c r="G28" s="16">
         <v>1.57</v>
       </c>
-      <c r="W28" s="33"/>
-      <c r="X28" s="43"/>
-      <c r="Y28" s="43"/>
-      <c r="Z28" s="43"/>
+      <c r="W28" s="32"/>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="42"/>
+      <c r="Z28" s="42"/>
     </row>
     <row r="29" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C29" s="8"/>
+      <c r="C29" s="47"/>
       <c r="D29" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>0.2</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="9">
         <v>3.59</v>
       </c>
-      <c r="G29" s="17">
+      <c r="G29" s="16">
         <v>1.08</v>
       </c>
-      <c r="H29" s="23" t="s">
+      <c r="H29" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="W29" s="33"/>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="43"/>
-      <c r="Z29" s="43"/>
+      <c r="W29" s="32"/>
+      <c r="X29" s="42"/>
+      <c r="Y29" s="42"/>
+      <c r="Z29" s="42"/>
     </row>
     <row r="30" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W30" s="33"/>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="43"/>
-      <c r="Z30" s="43"/>
+      <c r="W30" s="32"/>
+      <c r="X30" s="42"/>
+      <c r="Y30" s="42"/>
+      <c r="Z30" s="42"/>
     </row>
     <row r="31" spans="3:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="47" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
         <v>0</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="9">
         <v>8.6199999999999992</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="9">
         <v>8.7200000000000006</v>
       </c>
-      <c r="G31" s="17">
+      <c r="G31" s="16">
         <v>8.4</v>
       </c>
-      <c r="H31" s="23">
+      <c r="H31" s="22">
         <v>8.3800000000000008</v>
       </c>
-      <c r="I31" s="30">
+      <c r="I31" s="29">
         <v>8.4</v>
       </c>
-      <c r="J31" s="30">
+      <c r="J31" s="29">
         <v>8.5500000000000007</v>
       </c>
-      <c r="K31" s="30">
+      <c r="K31" s="29">
         <v>8.4</v>
       </c>
-      <c r="L31" s="30">
+      <c r="L31" s="29">
         <v>8.4</v>
       </c>
-      <c r="M31" s="30">
+      <c r="M31" s="29">
         <v>8.5500000000000007</v>
       </c>
-      <c r="N31" s="30">
+      <c r="N31" s="29">
         <v>8.44</v>
       </c>
-      <c r="O31" s="30">
+      <c r="O31" s="29">
         <v>8.4</v>
       </c>
-      <c r="P31" s="30">
+      <c r="P31" s="29">
         <v>8.5500000000000007</v>
       </c>
-      <c r="Q31" s="30">
+      <c r="Q31" s="29">
         <v>8.44</v>
       </c>
-      <c r="R31" s="38">
+      <c r="R31" s="37">
         <v>8.44</v>
       </c>
-      <c r="S31" s="38">
+      <c r="S31" s="37">
         <v>8.44</v>
       </c>
-      <c r="T31" s="38">
+      <c r="T31" s="37">
         <v>8.44</v>
       </c>
-      <c r="U31" s="30">
+      <c r="U31" s="29">
         <v>8.44</v>
       </c>
-      <c r="V31" s="30">
+      <c r="V31" s="29">
         <v>8.44</v>
       </c>
-      <c r="W31" s="33">
+      <c r="W31" s="32">
         <v>8.44</v>
       </c>
-      <c r="X31" s="43">
+      <c r="X31" s="42">
         <v>8.44</v>
       </c>
-      <c r="Y31" s="43">
+      <c r="Y31" s="42">
         <v>8.44</v>
       </c>
-      <c r="Z31" s="43">
+      <c r="Z31" s="42">
         <v>8.44</v>
       </c>
     </row>
     <row r="32" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C32" s="8"/>
+      <c r="C32" s="47"/>
       <c r="D32" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="9">
         <v>7.8</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="9">
         <v>3.62</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="16">
         <v>2.58</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="22">
         <v>2.67</v>
       </c>
-      <c r="I32" s="30">
+      <c r="I32" s="29">
         <v>2.48</v>
       </c>
-      <c r="J32" s="30">
+      <c r="J32" s="29">
         <v>2.83</v>
       </c>
-      <c r="K32" s="30">
+      <c r="K32" s="29">
         <v>1.17</v>
       </c>
-      <c r="L32" s="30">
+      <c r="L32" s="29">
         <v>1.55</v>
       </c>
-      <c r="M32" s="30">
+      <c r="M32" s="29">
         <v>2.8</v>
       </c>
-      <c r="N32" s="30">
+      <c r="N32" s="29">
         <v>2.0699999999999998</v>
       </c>
-      <c r="O32" s="30">
+      <c r="O32" s="29">
         <v>1.27</v>
       </c>
-      <c r="P32" s="30">
+      <c r="P32" s="29">
         <v>1.1599999999999999</v>
       </c>
-      <c r="Q32" s="30">
+      <c r="Q32" s="29">
         <v>1.56</v>
       </c>
-      <c r="R32" s="38">
+      <c r="R32" s="37">
         <v>2.12</v>
       </c>
-      <c r="S32" s="38">
+      <c r="S32" s="37">
         <v>1.75</v>
       </c>
-      <c r="T32" s="38">
+      <c r="T32" s="37">
         <v>1.1499999999999999</v>
       </c>
-      <c r="U32" s="30">
+      <c r="U32" s="29">
         <v>1.3</v>
       </c>
-      <c r="V32" s="30">
+      <c r="V32" s="29">
         <v>2.2650000000000001</v>
       </c>
-      <c r="W32" s="33">
+      <c r="W32" s="32">
         <v>1.6140000000000001</v>
       </c>
-      <c r="X32" s="43">
+      <c r="X32" s="42">
         <v>1.867</v>
       </c>
-      <c r="Y32" s="43">
+      <c r="Y32" s="42">
         <v>1</v>
       </c>
-      <c r="Z32" s="43">
+      <c r="Z32" s="42">
         <v>1.99</v>
       </c>
     </row>
     <row r="33" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C33" s="8"/>
+      <c r="C33" s="47"/>
       <c r="D33" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="9">
         <v>4.57</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="9">
         <v>6.97</v>
       </c>
-      <c r="G33" s="17">
+      <c r="G33" s="16">
         <v>2.2599999999999998</v>
       </c>
-      <c r="W33" s="33"/>
-      <c r="X33" s="43"/>
-      <c r="Y33" s="43"/>
-      <c r="Z33" s="43"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="42"/>
+      <c r="Z33" s="42"/>
     </row>
     <row r="34" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C34" s="8"/>
+      <c r="C34" s="47"/>
       <c r="D34" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="9">
         <v>0.3</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="9">
         <v>2.61</v>
       </c>
-      <c r="G34" s="17">
+      <c r="G34" s="16">
         <v>0.97</v>
       </c>
-      <c r="H34" s="23">
+      <c r="H34" s="22">
         <v>1.89</v>
       </c>
-      <c r="W34" s="33"/>
-      <c r="X34" s="43"/>
-      <c r="Y34" s="43"/>
-      <c r="Z34" s="43"/>
+      <c r="W34" s="32"/>
+      <c r="X34" s="42"/>
+      <c r="Y34" s="42"/>
+      <c r="Z34" s="42"/>
     </row>
     <row r="35" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C35" s="2"/>
-      <c r="W35" s="33"/>
-      <c r="X35" s="43"/>
-      <c r="Y35" s="43"/>
-      <c r="Z35" s="43"/>
+      <c r="W35" s="32"/>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="42"/>
+      <c r="Z35" s="42"/>
     </row>
     <row r="36" spans="3:26" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="47" t="s">
         <v>62</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="9">
         <f>5.84/2</f>
         <v>2.92</v>
       </c>
-      <c r="G36" s="17">
-        <v>0</v>
-      </c>
-      <c r="H36" s="23">
-        <v>0</v>
-      </c>
-      <c r="W36" s="33"/>
-      <c r="X36" s="43"/>
-      <c r="Y36" s="43"/>
-      <c r="Z36" s="43"/>
+      <c r="G36" s="16">
+        <v>0</v>
+      </c>
+      <c r="H36" s="22">
+        <v>0</v>
+      </c>
+      <c r="W36" s="32"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="42"/>
+      <c r="Z36" s="42"/>
     </row>
     <row r="37" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C37" s="8"/>
+      <c r="C37" s="47"/>
       <c r="D37" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="9">
         <f>0.332/2</f>
         <v>0.16600000000000001</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="12">
         <f>3.574/2</f>
         <v>1.7869999999999999</v>
       </c>
-      <c r="G37" s="19">
+      <c r="G37" s="18">
         <f>9.55/5</f>
         <v>1.9100000000000001</v>
       </c>
-      <c r="H37" s="26">
+      <c r="H37" s="25">
         <f>26.27/10</f>
         <v>2.6269999999999998</v>
       </c>
-      <c r="N37" s="30">
+      <c r="N37" s="29">
         <v>3.0049999999999999</v>
       </c>
-      <c r="O37" s="28">
+      <c r="O37" s="27">
         <v>2.09</v>
       </c>
-      <c r="P37" s="28">
+      <c r="P37" s="27">
         <v>2.4609999999999999</v>
       </c>
-      <c r="Q37" s="28">
+      <c r="Q37" s="27">
         <f>60.15/20</f>
         <v>3.0074999999999998</v>
       </c>
-      <c r="R37" s="40">
+      <c r="R37" s="39">
         <v>4.7699999999999996</v>
       </c>
-      <c r="S37" s="40">
+      <c r="S37" s="39">
         <v>3.238</v>
       </c>
-      <c r="T37" s="40">
+      <c r="T37" s="39">
         <v>1.877</v>
       </c>
-      <c r="U37" s="28">
+      <c r="U37" s="27">
         <v>2.1269999999999998</v>
       </c>
-      <c r="V37" s="28">
+      <c r="V37" s="27">
         <v>4.16</v>
       </c>
-      <c r="W37" s="35">
+      <c r="W37" s="34">
         <v>3.1269999999999998</v>
       </c>
-      <c r="X37" s="45">
+      <c r="X37" s="44">
         <v>3.2389999999999999</v>
       </c>
-      <c r="Y37" s="45">
+      <c r="Y37" s="44">
         <v>1.64</v>
       </c>
-      <c r="Z37" s="45">
+      <c r="Z37" s="44">
         <v>3.6349999999999998</v>
       </c>
     </row>
     <row r="38" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C38" s="8"/>
+      <c r="C38" s="47"/>
       <c r="D38" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="12">
         <f>2.62/2</f>
         <v>1.31</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F38" s="13">
         <f>5.56/2</f>
         <v>2.78</v>
       </c>
-      <c r="G38" s="17">
+      <c r="G38" s="16">
         <f>19.377/5</f>
         <v>3.8754</v>
       </c>
-      <c r="W38" s="33"/>
-      <c r="X38" s="43"/>
-      <c r="Y38" s="43"/>
-      <c r="Z38" s="43"/>
+      <c r="W38" s="32"/>
+      <c r="X38" s="42"/>
+      <c r="Y38" s="42"/>
+      <c r="Z38" s="42"/>
     </row>
     <row r="39" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C39" s="8"/>
+      <c r="C39" s="47"/>
       <c r="D39" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="9">
         <f>0.281/2</f>
         <v>0.14050000000000001</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="13">
         <f>0.77/2</f>
         <v>0.38500000000000001</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G39" s="16">
         <f>2.785/5</f>
         <v>0.55700000000000005</v>
       </c>
-      <c r="W39" s="33"/>
-      <c r="X39" s="43"/>
-      <c r="Y39" s="43"/>
-      <c r="Z39" s="43"/>
+      <c r="W39" s="32"/>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
+      <c r="Z39" s="42"/>
     </row>
     <row r="40" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C40" s="2"/>
-      <c r="F40" s="13"/>
-      <c r="W40" s="33"/>
-      <c r="X40" s="43"/>
-      <c r="Y40" s="43"/>
-      <c r="Z40" s="43"/>
+      <c r="F40" s="12"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
+      <c r="Z40" s="42"/>
     </row>
     <row r="41" spans="3:26" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="47" t="s">
         <v>56</v>
       </c>
       <c r="D41" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="9">
         <f>E21*E36</f>
         <v>14.891999999999999</v>
       </c>
-      <c r="G41" s="20">
+      <c r="G41" s="19">
         <f>G21*G36</f>
         <v>0</v>
       </c>
-      <c r="H41" s="29">
+      <c r="H41" s="28">
         <f>H21*H36</f>
         <v>0</v>
       </c>
-      <c r="I41" s="30">
+      <c r="I41" s="29">
         <f t="shared" ref="I41:Q41" si="0">I21*I36</f>
         <v>0</v>
       </c>
-      <c r="J41" s="30">
+      <c r="J41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K41" s="30">
+      <c r="K41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L41" s="30">
+      <c r="L41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M41" s="30">
+      <c r="M41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N41" s="30">
+      <c r="N41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O41" s="30">
+      <c r="O41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P41" s="30">
+      <c r="P41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="30">
+      <c r="Q41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R41" s="38">
+      <c r="R41" s="37">
         <f t="shared" ref="R41" si="1">R21*R36</f>
         <v>0</v>
       </c>
-      <c r="S41" s="38">
+      <c r="S41" s="37">
         <f t="shared" ref="S41:T41" si="2">S21*S36</f>
         <v>0</v>
       </c>
-      <c r="T41" s="38">
+      <c r="T41" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U41" s="30">
-        <f>U21*U36</f>
-        <v>0</v>
-      </c>
-      <c r="V41" s="30">
-        <f>V21*V36</f>
-        <v>0</v>
-      </c>
-      <c r="W41" s="33">
-        <v>0</v>
-      </c>
-      <c r="X41" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="43">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="43">
+      <c r="U41" s="29">
+        <f t="shared" ref="U41:V44" si="3">U21*U36</f>
+        <v>0</v>
+      </c>
+      <c r="V41" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W41" s="32">
+        <v>0</v>
+      </c>
+      <c r="X41" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C42" s="8"/>
+      <c r="C42" s="47"/>
       <c r="D42" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="9">
         <f>E22*E37</f>
         <v>12.929740000000001</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F42" s="12">
         <f>F22*F37</f>
         <v>157.43469999999999</v>
       </c>
-      <c r="G42" s="19">
-        <f t="shared" ref="G42:Q42" si="3">G22*G37</f>
+      <c r="G42" s="18">
+        <f t="shared" ref="G42:Q42" si="4">G22*G37</f>
         <v>164.833</v>
       </c>
-      <c r="H42" s="26">
+      <c r="H42" s="25">
+        <f t="shared" si="4"/>
+        <v>185.46619999999996</v>
+      </c>
+      <c r="I42" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L42" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N42" s="29">
+        <f t="shared" si="4"/>
+        <v>68.213499999999996</v>
+      </c>
+      <c r="O42" s="27">
+        <f t="shared" si="4"/>
+        <v>176.81399999999996</v>
+      </c>
+      <c r="P42" s="27">
+        <f t="shared" si="4"/>
+        <v>188.7587</v>
+      </c>
+      <c r="Q42" s="27">
+        <f t="shared" si="4"/>
+        <v>257.14125000000001</v>
+      </c>
+      <c r="R42" s="39">
+        <f t="shared" ref="R42" si="5">R22*R37</f>
+        <v>286.2</v>
+      </c>
+      <c r="S42" s="39">
+        <f t="shared" ref="S42:T42" si="6">S22*S37</f>
+        <v>297.89600000000002</v>
+      </c>
+      <c r="T42" s="39">
+        <f t="shared" si="6"/>
+        <v>146.40600000000001</v>
+      </c>
+      <c r="U42" s="27">
         <f t="shared" si="3"/>
-        <v>185.46619999999996</v>
-      </c>
-      <c r="I42" s="30">
+        <v>176.54099999999997</v>
+      </c>
+      <c r="V42" s="27">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J42" s="30">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K42" s="30">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L42" s="30">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M42" s="30">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N42" s="30">
-        <f t="shared" si="3"/>
-        <v>68.213499999999996</v>
-      </c>
-      <c r="O42" s="28">
-        <f t="shared" si="3"/>
-        <v>176.81399999999996</v>
-      </c>
-      <c r="P42" s="28">
-        <f t="shared" si="3"/>
-        <v>188.7587</v>
-      </c>
-      <c r="Q42" s="28">
-        <f t="shared" si="3"/>
-        <v>257.14125000000001</v>
-      </c>
-      <c r="R42" s="40">
-        <f t="shared" ref="R42" si="4">R22*R37</f>
-        <v>286.2</v>
-      </c>
-      <c r="S42" s="40">
-        <f t="shared" ref="S42:T42" si="5">S22*S37</f>
-        <v>297.89600000000002</v>
-      </c>
-      <c r="T42" s="40">
-        <f t="shared" si="5"/>
-        <v>146.40600000000001</v>
-      </c>
-      <c r="U42" s="28">
-        <f>U22*U37</f>
-        <v>176.54099999999997</v>
-      </c>
-      <c r="V42" s="28">
-        <f>V22*V37</f>
         <v>375.77280000000002</v>
       </c>
-      <c r="W42" s="28">
+      <c r="W42" s="27">
         <f>W22*W37</f>
         <v>269.95390999999995</v>
       </c>
-      <c r="X42" s="40">
-        <f t="shared" ref="X42:Z42" si="6">X22*X37</f>
+      <c r="X42" s="39">
+        <f t="shared" ref="X42:Z42" si="7">X22*X37</f>
         <v>259.12</v>
       </c>
-      <c r="Y42" s="40">
-        <f t="shared" si="6"/>
+      <c r="Y42" s="39">
+        <f t="shared" si="7"/>
         <v>136.12</v>
       </c>
-      <c r="Z42" s="40">
-        <f t="shared" si="6"/>
+      <c r="Z42" s="39">
+        <f t="shared" si="7"/>
         <v>283.52999999999997</v>
       </c>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C43" s="8"/>
+      <c r="C43" s="47"/>
       <c r="D43" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="12">
         <f>E23*E38</f>
         <v>41.789000000000001</v>
       </c>
-      <c r="F43" s="14">
+      <c r="F43" s="13">
         <f>F23*F38</f>
         <v>43.256799999999998</v>
       </c>
-      <c r="G43" s="20">
-        <f t="shared" ref="G43:Q43" si="7">G23*G38</f>
+      <c r="G43" s="19">
+        <f t="shared" ref="G43:Q43" si="8">G23*G38</f>
         <v>18.989460000000001</v>
       </c>
-      <c r="H43" s="29">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="O43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="R43" s="38">
-        <f t="shared" ref="R43" si="8">R23*R38</f>
-        <v>0</v>
-      </c>
-      <c r="S43" s="38">
-        <f t="shared" ref="S43:T43" si="9">S23*S38</f>
-        <v>0</v>
-      </c>
-      <c r="T43" s="38">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="U43" s="30">
-        <f>U23*U38</f>
-        <v>0</v>
-      </c>
-      <c r="V43" s="30">
-        <f>V23*V38</f>
-        <v>0</v>
-      </c>
-      <c r="W43" s="33">
-        <v>0</v>
-      </c>
-      <c r="X43" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="43">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="43">
+      <c r="H43" s="28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R43" s="37">
+        <f t="shared" ref="R43" si="9">R23*R38</f>
+        <v>0</v>
+      </c>
+      <c r="S43" s="37">
+        <f t="shared" ref="S43:T43" si="10">S23*S38</f>
+        <v>0</v>
+      </c>
+      <c r="T43" s="37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U43" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V43" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W43" s="32">
+        <v>0</v>
+      </c>
+      <c r="X43" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C44" s="8"/>
+      <c r="C44" s="47"/>
       <c r="D44" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="9">
         <f>E24*E39</f>
         <v>12.01275</v>
       </c>
-      <c r="F44" s="14">
+      <c r="F44" s="13">
         <f>F24*F39</f>
         <v>2.6565000000000003</v>
       </c>
-      <c r="G44" s="20">
-        <f t="shared" ref="G44:Q44" si="10">G24*G39</f>
+      <c r="G44" s="19">
+        <f t="shared" ref="G44:Q44" si="11">G24*G39</f>
         <v>30.913500000000003</v>
       </c>
-      <c r="H44" s="29">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="N44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="O44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q44" s="30">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="R44" s="38">
-        <f t="shared" ref="R44" si="11">R24*R39</f>
-        <v>0</v>
-      </c>
-      <c r="S44" s="38">
-        <f t="shared" ref="S44:T44" si="12">S24*S39</f>
-        <v>0</v>
-      </c>
-      <c r="T44" s="38">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="U44" s="30">
-        <f>U24*U39</f>
-        <v>0</v>
-      </c>
-      <c r="V44" s="30">
-        <f>V24*V39</f>
-        <v>0</v>
-      </c>
-      <c r="W44" s="33">
-        <v>0</v>
-      </c>
-      <c r="X44" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="43">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="43">
+      <c r="H44" s="28">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R44" s="37">
+        <f t="shared" ref="R44" si="12">R24*R39</f>
+        <v>0</v>
+      </c>
+      <c r="S44" s="37">
+        <f t="shared" ref="S44:T44" si="13">S24*S39</f>
+        <v>0</v>
+      </c>
+      <c r="T44" s="37">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="U44" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V44" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W44" s="32">
+        <v>0</v>
+      </c>
+      <c r="X44" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C45" s="2"/>
-      <c r="F45" s="13"/>
-      <c r="W45" s="33"/>
-      <c r="X45" s="43"/>
-      <c r="Y45" s="43"/>
-      <c r="Z45" s="43"/>
+      <c r="F45" s="12"/>
+      <c r="W45" s="32"/>
+      <c r="X45" s="42"/>
+      <c r="Y45" s="42"/>
+      <c r="Z45" s="42"/>
     </row>
     <row r="46" spans="3:26" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="6"/>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="G46" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="32" t="s">
+      <c r="I46" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="32" t="s">
+      <c r="J46" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="K46" s="32" t="s">
+      <c r="K46" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="L46" s="32" t="s">
+      <c r="L46" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="M46" s="32" t="s">
+      <c r="M46" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="N46" s="32" t="s">
+      <c r="N46" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="O46" s="32" t="s">
+      <c r="O46" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="P46" s="32" t="s">
+      <c r="P46" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="Q46" s="32" t="s">
+      <c r="Q46" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R46" s="42" t="s">
+      <c r="R46" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="S46" s="42" t="s">
+      <c r="S46" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="T46" s="42" t="s">
+      <c r="T46" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="U46" s="32" t="s">
+      <c r="U46" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="V46" s="32" t="s">
+      <c r="V46" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="W46" s="37" t="s">
+      <c r="W46" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="X46" s="47" t="s">
+      <c r="X46" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="Y46" s="47" t="s">
+      <c r="Y46" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="Z46" s="47" t="s">
+      <c r="Z46" s="46" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3043,207 +3043,207 @@
         <v>37</v>
       </c>
       <c r="D47" s="6"/>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H47" s="25" t="s">
+      <c r="H47" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="42"/>
-      <c r="S47" s="42"/>
-      <c r="T47" s="42"/>
-      <c r="U47" s="32"/>
-      <c r="V47" s="32"/>
-      <c r="W47" s="37"/>
-      <c r="X47" s="47"/>
-      <c r="Y47" s="47"/>
-      <c r="Z47" s="47"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="41"/>
+      <c r="S47" s="41"/>
+      <c r="T47" s="41"/>
+      <c r="U47" s="31"/>
+      <c r="V47" s="31"/>
+      <c r="W47" s="36"/>
+      <c r="X47" s="46"/>
+      <c r="Y47" s="46"/>
+      <c r="Z47" s="46"/>
     </row>
     <row r="48" spans="3:26" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D48" s="6"/>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H48" s="25" t="s">
+      <c r="H48" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="32"/>
-      <c r="R48" s="42"/>
-      <c r="S48" s="42"/>
-      <c r="T48" s="42"/>
-      <c r="U48" s="32"/>
-      <c r="V48" s="32"/>
-      <c r="W48" s="37"/>
-      <c r="X48" s="47"/>
-      <c r="Y48" s="47"/>
-      <c r="Z48" s="47"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="O48" s="31"/>
+      <c r="P48" s="31"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="41"/>
+      <c r="S48" s="41"/>
+      <c r="T48" s="41"/>
+      <c r="U48" s="31"/>
+      <c r="V48" s="31"/>
+      <c r="W48" s="36"/>
+      <c r="X48" s="46"/>
+      <c r="Y48" s="46"/>
+      <c r="Z48" s="46"/>
     </row>
     <row r="49" spans="3:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C49" s="5"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="32"/>
-      <c r="R49" s="42"/>
-      <c r="S49" s="42"/>
-      <c r="T49" s="42"/>
-      <c r="U49" s="32"/>
-      <c r="V49" s="32"/>
-      <c r="W49" s="37"/>
-      <c r="X49" s="47"/>
-      <c r="Y49" s="47"/>
-      <c r="Z49" s="47"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="41"/>
+      <c r="S49" s="41"/>
+      <c r="T49" s="41"/>
+      <c r="U49" s="31"/>
+      <c r="V49" s="31"/>
+      <c r="W49" s="36"/>
+      <c r="X49" s="46"/>
+      <c r="Y49" s="46"/>
+      <c r="Z49" s="46"/>
     </row>
     <row r="50" spans="3:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C50" s="5"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="32"/>
-      <c r="N50" s="32"/>
-      <c r="O50" s="32"/>
-      <c r="P50" s="32"/>
-      <c r="Q50" s="32"/>
-      <c r="R50" s="42"/>
-      <c r="S50" s="42"/>
-      <c r="T50" s="42"/>
-      <c r="U50" s="32"/>
-      <c r="V50" s="32"/>
-      <c r="W50" s="37"/>
-      <c r="X50" s="47"/>
-      <c r="Y50" s="47"/>
-      <c r="Z50" s="47"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="31"/>
+      <c r="P50" s="31"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="41"/>
+      <c r="S50" s="41"/>
+      <c r="T50" s="41"/>
+      <c r="U50" s="31"/>
+      <c r="V50" s="31"/>
+      <c r="W50" s="36"/>
+      <c r="X50" s="46"/>
+      <c r="Y50" s="46"/>
+      <c r="Z50" s="46"/>
     </row>
     <row r="51" spans="3:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C51" s="5"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
-      <c r="O51" s="32"/>
-      <c r="P51" s="32"/>
-      <c r="Q51" s="32"/>
-      <c r="R51" s="42"/>
-      <c r="S51" s="42"/>
-      <c r="T51" s="42"/>
-      <c r="U51" s="32"/>
-      <c r="V51" s="32"/>
-      <c r="W51" s="37"/>
-      <c r="X51" s="47"/>
-      <c r="Y51" s="47"/>
-      <c r="Z51" s="47"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="31"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="31"/>
+      <c r="M51" s="31"/>
+      <c r="N51" s="31"/>
+      <c r="O51" s="31"/>
+      <c r="P51" s="31"/>
+      <c r="Q51" s="31"/>
+      <c r="R51" s="41"/>
+      <c r="S51" s="41"/>
+      <c r="T51" s="41"/>
+      <c r="U51" s="31"/>
+      <c r="V51" s="31"/>
+      <c r="W51" s="36"/>
+      <c r="X51" s="46"/>
+      <c r="Y51" s="46"/>
+      <c r="Z51" s="46"/>
     </row>
     <row r="52" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W52" s="33"/>
-      <c r="X52" s="43"/>
-      <c r="Y52" s="43"/>
-      <c r="Z52" s="43"/>
+      <c r="W52" s="32"/>
+      <c r="X52" s="42"/>
+      <c r="Y52" s="42"/>
+      <c r="Z52" s="42"/>
     </row>
     <row r="53" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W53" s="33"/>
-      <c r="X53" s="43"/>
-      <c r="Y53" s="43"/>
-      <c r="Z53" s="43"/>
+      <c r="W53" s="32"/>
+      <c r="X53" s="42"/>
+      <c r="Y53" s="42"/>
+      <c r="Z53" s="42"/>
     </row>
     <row r="54" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W54" s="33"/>
-      <c r="X54" s="43"/>
-      <c r="Y54" s="43"/>
-      <c r="Z54" s="43"/>
+      <c r="W54" s="32"/>
+      <c r="X54" s="42"/>
+      <c r="Y54" s="42"/>
+      <c r="Z54" s="42"/>
     </row>
     <row r="55" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W55" s="33"/>
-      <c r="X55" s="43"/>
-      <c r="Y55" s="43"/>
-      <c r="Z55" s="43"/>
+      <c r="W55" s="32"/>
+      <c r="X55" s="42"/>
+      <c r="Y55" s="42"/>
+      <c r="Z55" s="42"/>
     </row>
     <row r="56" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W56" s="33"/>
-      <c r="X56" s="43"/>
-      <c r="Y56" s="43"/>
-      <c r="Z56" s="43"/>
+      <c r="W56" s="32"/>
+      <c r="X56" s="42"/>
+      <c r="Y56" s="42"/>
+      <c r="Z56" s="42"/>
     </row>
     <row r="57" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W57" s="33"/>
-      <c r="X57" s="43"/>
-      <c r="Y57" s="43"/>
-      <c r="Z57" s="43"/>
+      <c r="W57" s="32"/>
+      <c r="X57" s="42"/>
+      <c r="Y57" s="42"/>
+      <c r="Z57" s="42"/>
     </row>
     <row r="58" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W58" s="33"/>
-      <c r="X58" s="43"/>
-      <c r="Y58" s="43"/>
-      <c r="Z58" s="43"/>
+      <c r="W58" s="32"/>
+      <c r="X58" s="42"/>
+      <c r="Y58" s="42"/>
+      <c r="Z58" s="42"/>
     </row>
     <row r="59" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W59" s="33"/>
-      <c r="X59" s="43"/>
-      <c r="Y59" s="43"/>
-      <c r="Z59" s="43"/>
+      <c r="W59" s="32"/>
+      <c r="X59" s="42"/>
+      <c r="Y59" s="42"/>
+      <c r="Z59" s="42"/>
     </row>
     <row r="60" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="W60" s="33"/>
-      <c r="X60" s="43"/>
-      <c r="Y60" s="43"/>
-      <c r="Z60" s="43"/>
+      <c r="W60" s="32"/>
+      <c r="X60" s="42"/>
+      <c r="Y60" s="42"/>
+      <c r="Z60" s="42"/>
     </row>
     <row r="61" spans="3:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="W61" s="33"/>
-      <c r="X61" s="43"/>
-      <c r="Y61" s="43"/>
-      <c r="Z61" s="43"/>
+      <c r="W61" s="32"/>
+      <c r="X61" s="42"/>
+      <c r="Y61" s="42"/>
+      <c r="Z61" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>